<commit_message>
test pages and fix bug
Signed-off-by: yangjiawei <yangjiawei@xiaomi.com>
</commit_message>
<xml_diff>
--- a/uploads/user/老师.xlsx
+++ b/uploads/user/老师.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>学号</t>
   </si>
@@ -34,6 +34,33 @@
   </si>
   <si>
     <t>男</t>
+  </si>
+  <si>
+    <t>谭火彬</t>
+  </si>
+  <si>
+    <t>刘辰泪</t>
+  </si>
+  <si>
+    <t>刘梓晨</t>
+  </si>
+  <si>
+    <t>蛇精病</t>
+  </si>
+  <si>
+    <t>女</t>
+  </si>
+  <si>
+    <t>溜了溜了</t>
+  </si>
+  <si>
+    <t>极乐净土</t>
+  </si>
+  <si>
+    <t>林广艳</t>
+  </si>
+  <si>
+    <t>贾经东</t>
   </si>
 </sst>
 </file>
@@ -41,10 +68,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -56,6 +83,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -63,61 +105,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -129,6 +171,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -137,11 +187,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,47 +211,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,49 +235,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,31 +361,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,97 +403,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,6 +426,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,50 +455,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,19 +482,47 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,145 +534,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1002,17 +1029,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9.375"/>
-    <col min="4" max="4" width="11.5"/>
-    <col min="5" max="5" width="12.625"/>
+    <col min="4" max="5" width="12.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1031,7 +1057,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>711001</v>
+        <v>721001</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1041,6 +1067,118 @@
       </c>
       <c r="D2">
         <v>911</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>721002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>13552755185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>721003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>721004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>721005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>721006</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>721007</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>721008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>721009</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>919</v>
       </c>
     </row>
   </sheetData>

</xml_diff>